<commit_message>
Listing détaillé des cours
</commit_message>
<xml_diff>
--- a/M1/Optimisation stochastique/Projet/Curriculum.xlsx
+++ b/M1/Optimisation stochastique/Projet/Curriculum.xlsx
@@ -8,20 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Workspaces\Cours\M1\Optimisation stochastique\Projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D7495AB-EEB1-4DB2-832E-3C811AA5F8E8}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50390BF5-29CF-47D3-B1BB-1E6B80E200A7}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11850" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="-R- List of courses" sheetId="1" r:id="rId1"/>
     <sheet name="L0" sheetId="2" r:id="rId2"/>
+    <sheet name="L1CE" sheetId="3" r:id="rId3"/>
+    <sheet name="L1CS" sheetId="4" r:id="rId4"/>
+    <sheet name="L1GE" sheetId="5" r:id="rId5"/>
+    <sheet name="L1OG" sheetId="6" r:id="rId6"/>
+    <sheet name="Total" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="117">
   <si>
     <t>FOUNDATION YEAR</t>
   </si>
@@ -348,9 +353,6 @@
     <t>NB_COURS_L0</t>
   </si>
   <si>
-    <t>NB_COURS_COMMUN_L1</t>
-  </si>
-  <si>
     <t>NB_COURS_CE</t>
   </si>
   <si>
@@ -361,6 +363,21 @@
   </si>
   <si>
     <t>NB_COURS_OG</t>
+  </si>
+  <si>
+    <t>L1CE</t>
+  </si>
+  <si>
+    <t>L1CS</t>
+  </si>
+  <si>
+    <t>L1GE</t>
+  </si>
+  <si>
+    <t>L1OG</t>
+  </si>
+  <si>
+    <t>NB_GROUPES_PAR_SPE</t>
   </si>
 </sst>
 </file>
@@ -1093,7 +1110,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="221">
+  <cellXfs count="222">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -1634,80 +1651,44 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="13" fillId="2" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="13" fillId="6" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="7" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="8" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="49" fontId="11" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="13" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="13" fillId="6" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1715,6 +1696,43 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="8" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="13" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="13" fillId="7" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="13" fillId="2" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="6" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2001,8 +2019,8 @@
   </sheetPr>
   <dimension ref="A1:AI1014"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="O95" sqref="O95:P95"/>
+    <sheetView topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="J74" sqref="J74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -2053,11 +2071,11 @@
       <c r="AI1" s="3"/>
     </row>
     <row r="2" spans="1:35" ht="15.75">
-      <c r="A2" s="210" t="s">
+      <c r="A2" s="183" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2"/>
-      <c r="C2" s="216" t="s">
+      <c r="C2" s="195" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="196"/>
@@ -2094,22 +2112,22 @@
       <c r="AI2" s="3"/>
     </row>
     <row r="3" spans="1:35" ht="15.75">
-      <c r="A3" s="200"/>
+      <c r="A3" s="184"/>
       <c r="B3" s="2"/>
-      <c r="C3" s="215" t="s">
+      <c r="C3" s="193" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="200"/>
-      <c r="E3" s="200"/>
-      <c r="F3" s="200"/>
-      <c r="G3" s="200"/>
-      <c r="H3" s="200"/>
-      <c r="I3" s="200"/>
-      <c r="J3" s="200"/>
-      <c r="K3" s="200"/>
-      <c r="L3" s="200"/>
-      <c r="M3" s="200"/>
-      <c r="N3" s="201"/>
+      <c r="D3" s="184"/>
+      <c r="E3" s="184"/>
+      <c r="F3" s="184"/>
+      <c r="G3" s="184"/>
+      <c r="H3" s="184"/>
+      <c r="I3" s="184"/>
+      <c r="J3" s="184"/>
+      <c r="K3" s="184"/>
+      <c r="L3" s="184"/>
+      <c r="M3" s="184"/>
+      <c r="N3" s="194"/>
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
@@ -2133,22 +2151,22 @@
       <c r="AI3" s="3"/>
     </row>
     <row r="4" spans="1:35" ht="15.75">
-      <c r="A4" s="200"/>
+      <c r="A4" s="184"/>
       <c r="B4" s="4"/>
-      <c r="C4" s="217" t="s">
+      <c r="C4" s="198" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="183"/>
-      <c r="E4" s="183"/>
-      <c r="F4" s="183"/>
-      <c r="G4" s="183"/>
-      <c r="H4" s="183"/>
-      <c r="I4" s="183"/>
-      <c r="J4" s="183"/>
-      <c r="K4" s="183"/>
-      <c r="L4" s="183"/>
-      <c r="M4" s="183"/>
-      <c r="N4" s="184"/>
+      <c r="D4" s="199"/>
+      <c r="E4" s="199"/>
+      <c r="F4" s="199"/>
+      <c r="G4" s="199"/>
+      <c r="H4" s="199"/>
+      <c r="I4" s="199"/>
+      <c r="J4" s="199"/>
+      <c r="K4" s="199"/>
+      <c r="L4" s="199"/>
+      <c r="M4" s="199"/>
+      <c r="N4" s="200"/>
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
       <c r="Q4" s="3"/>
@@ -2172,7 +2190,7 @@
       <c r="AI4" s="3"/>
     </row>
     <row r="5" spans="1:35" ht="35.25" customHeight="1">
-      <c r="A5" s="200"/>
+      <c r="A5" s="184"/>
       <c r="B5" s="5"/>
       <c r="C5" s="6" t="s">
         <v>4</v>
@@ -2225,7 +2243,7 @@
       <c r="AI5" s="12"/>
     </row>
     <row r="6" spans="1:35" ht="15.75">
-      <c r="A6" s="200"/>
+      <c r="A6" s="184"/>
       <c r="B6" s="13"/>
       <c r="C6" s="14" t="s">
         <v>12</v>
@@ -2270,7 +2288,7 @@
       <c r="AI6" s="12"/>
     </row>
     <row r="7" spans="1:35" ht="15.75">
-      <c r="A7" s="200"/>
+      <c r="A7" s="184"/>
       <c r="B7" s="13"/>
       <c r="C7" s="14" t="s">
         <v>14</v>
@@ -2315,7 +2333,7 @@
       <c r="AI7" s="12"/>
     </row>
     <row r="8" spans="1:35" ht="15.75">
-      <c r="A8" s="200"/>
+      <c r="A8" s="184"/>
       <c r="B8" s="13"/>
       <c r="C8" s="14" t="s">
         <v>16</v>
@@ -2360,7 +2378,7 @@
       <c r="AI8" s="12"/>
     </row>
     <row r="9" spans="1:35" ht="15.75">
-      <c r="A9" s="200"/>
+      <c r="A9" s="184"/>
       <c r="B9" s="13"/>
       <c r="C9" s="14" t="s">
         <v>18</v>
@@ -2406,7 +2424,7 @@
       <c r="AI9" s="12"/>
     </row>
     <row r="10" spans="1:35" ht="15.75">
-      <c r="A10" s="200"/>
+      <c r="A10" s="184"/>
       <c r="B10" s="13"/>
       <c r="C10" s="14" t="s">
         <v>19</v>
@@ -2453,7 +2471,7 @@
       <c r="AI10" s="12"/>
     </row>
     <row r="11" spans="1:35" ht="15.75">
-      <c r="A11" s="200"/>
+      <c r="A11" s="184"/>
       <c r="B11" s="13"/>
       <c r="C11" s="14" t="s">
         <v>21</v>
@@ -2500,7 +2518,7 @@
       <c r="AI11" s="12"/>
     </row>
     <row r="12" spans="1:35" ht="15.75">
-      <c r="A12" s="200"/>
+      <c r="A12" s="184"/>
       <c r="B12" s="13"/>
       <c r="C12" s="14" t="s">
         <v>23</v>
@@ -2545,12 +2563,12 @@
       <c r="AI12" s="12"/>
     </row>
     <row r="13" spans="1:35" ht="15.75">
-      <c r="A13" s="200"/>
+      <c r="A13" s="184"/>
       <c r="B13" s="38"/>
-      <c r="C13" s="191" t="s">
+      <c r="C13" s="186" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="192"/>
+      <c r="D13" s="187"/>
       <c r="E13" s="39">
         <f>SUM(E6:E12)</f>
         <v>20</v>
@@ -2561,15 +2579,15 @@
         <v>0</v>
       </c>
       <c r="H13" s="62">
-        <f t="shared" ref="H13:J13" si="0">SUM(H6:H12)</f>
+        <f>SUM(H6:H12)</f>
         <v>294</v>
       </c>
       <c r="I13" s="62">
-        <f t="shared" si="0"/>
+        <f>SUM(I6:I12)</f>
         <v>0</v>
       </c>
       <c r="J13" s="62">
-        <f t="shared" si="0"/>
+        <f>SUM(J6:J12)</f>
         <v>98</v>
       </c>
       <c r="K13" s="41"/>
@@ -2599,7 +2617,7 @@
       <c r="AI13" s="12"/>
     </row>
     <row r="14" spans="1:35" ht="34.5" customHeight="1">
-      <c r="A14" s="200"/>
+      <c r="A14" s="184"/>
       <c r="B14" s="44"/>
       <c r="C14" s="44"/>
       <c r="D14" s="45"/>
@@ -2636,9 +2654,9 @@
       <c r="AI14" s="12"/>
     </row>
     <row r="15" spans="1:35" ht="15.75">
-      <c r="A15" s="200"/>
+      <c r="A15" s="184"/>
       <c r="B15" s="2"/>
-      <c r="C15" s="216" t="s">
+      <c r="C15" s="195" t="s">
         <v>1</v>
       </c>
       <c r="D15" s="196"/>
@@ -2675,22 +2693,22 @@
       <c r="AI15" s="3"/>
     </row>
     <row r="16" spans="1:35" ht="15.75">
-      <c r="A16" s="200"/>
+      <c r="A16" s="184"/>
       <c r="B16" s="2"/>
-      <c r="C16" s="215" t="s">
+      <c r="C16" s="193" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="200"/>
-      <c r="E16" s="200"/>
-      <c r="F16" s="200"/>
-      <c r="G16" s="200"/>
-      <c r="H16" s="200"/>
-      <c r="I16" s="200"/>
-      <c r="J16" s="200"/>
-      <c r="K16" s="200"/>
-      <c r="L16" s="200"/>
-      <c r="M16" s="200"/>
-      <c r="N16" s="201"/>
+      <c r="D16" s="184"/>
+      <c r="E16" s="184"/>
+      <c r="F16" s="184"/>
+      <c r="G16" s="184"/>
+      <c r="H16" s="184"/>
+      <c r="I16" s="184"/>
+      <c r="J16" s="184"/>
+      <c r="K16" s="184"/>
+      <c r="L16" s="184"/>
+      <c r="M16" s="184"/>
+      <c r="N16" s="194"/>
       <c r="O16" s="3"/>
       <c r="P16" s="3"/>
       <c r="Q16" s="3"/>
@@ -2714,22 +2732,22 @@
       <c r="AI16" s="3"/>
     </row>
     <row r="17" spans="1:35" ht="15.75">
-      <c r="A17" s="200"/>
+      <c r="A17" s="184"/>
       <c r="B17" s="4"/>
-      <c r="C17" s="217" t="s">
+      <c r="C17" s="198" t="s">
         <v>27</v>
       </c>
-      <c r="D17" s="183"/>
-      <c r="E17" s="183"/>
-      <c r="F17" s="183"/>
-      <c r="G17" s="183"/>
-      <c r="H17" s="183"/>
-      <c r="I17" s="183"/>
-      <c r="J17" s="183"/>
-      <c r="K17" s="183"/>
-      <c r="L17" s="183"/>
-      <c r="M17" s="183"/>
-      <c r="N17" s="184"/>
+      <c r="D17" s="199"/>
+      <c r="E17" s="199"/>
+      <c r="F17" s="199"/>
+      <c r="G17" s="199"/>
+      <c r="H17" s="199"/>
+      <c r="I17" s="199"/>
+      <c r="J17" s="199"/>
+      <c r="K17" s="199"/>
+      <c r="L17" s="199"/>
+      <c r="M17" s="199"/>
+      <c r="N17" s="200"/>
       <c r="O17" s="3"/>
       <c r="P17" s="3"/>
       <c r="Q17" s="3"/>
@@ -2753,7 +2771,7 @@
       <c r="AI17" s="3"/>
     </row>
     <row r="18" spans="1:35" ht="43.5" customHeight="1">
-      <c r="A18" s="200"/>
+      <c r="A18" s="184"/>
       <c r="B18" s="5"/>
       <c r="C18" s="6" t="s">
         <v>4</v>
@@ -2806,15 +2824,15 @@
       <c r="AI18" s="12"/>
     </row>
     <row r="19" spans="1:35" ht="15.75">
-      <c r="A19" s="200"/>
+      <c r="A19" s="184"/>
       <c r="B19" s="50"/>
-      <c r="C19" s="214" t="s">
+      <c r="C19" s="192" t="s">
         <v>29</v>
       </c>
       <c r="D19" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="193">
+      <c r="E19" s="206">
         <v>4</v>
       </c>
       <c r="F19" s="52"/>
@@ -2853,13 +2871,13 @@
       <c r="AI19" s="12"/>
     </row>
     <row r="20" spans="1:35" ht="15.75">
-      <c r="A20" s="200"/>
+      <c r="A20" s="184"/>
       <c r="B20" s="50"/>
-      <c r="C20" s="208"/>
+      <c r="C20" s="191"/>
       <c r="D20" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="E20" s="194"/>
+      <c r="E20" s="207"/>
       <c r="F20" s="52"/>
       <c r="G20" s="52">
         <v>10</v>
@@ -2896,7 +2914,7 @@
       <c r="AI20" s="12"/>
     </row>
     <row r="21" spans="1:35" ht="15.75">
-      <c r="A21" s="200"/>
+      <c r="A21" s="184"/>
       <c r="B21" s="55"/>
       <c r="C21" s="56" t="s">
         <v>32</v>
@@ -2945,7 +2963,7 @@
       <c r="AI21" s="12"/>
     </row>
     <row r="22" spans="1:35" ht="15.75">
-      <c r="A22" s="200"/>
+      <c r="A22" s="184"/>
       <c r="B22" s="13"/>
       <c r="C22" s="14" t="s">
         <v>34</v>
@@ -2995,7 +3013,7 @@
       <c r="AI22" s="12"/>
     </row>
     <row r="23" spans="1:35" ht="15.75">
-      <c r="A23" s="200"/>
+      <c r="A23" s="184"/>
       <c r="B23" s="55"/>
       <c r="C23" s="56" t="s">
         <v>35</v>
@@ -3044,7 +3062,7 @@
       <c r="AI23" s="12"/>
     </row>
     <row r="24" spans="1:35" ht="15.75">
-      <c r="A24" s="200"/>
+      <c r="A24" s="184"/>
       <c r="B24" s="13"/>
       <c r="C24" s="14" t="s">
         <v>37</v>
@@ -3089,7 +3107,7 @@
       <c r="AI24" s="12"/>
     </row>
     <row r="25" spans="1:35" ht="15.75">
-      <c r="A25" s="200"/>
+      <c r="A25" s="184"/>
       <c r="B25" s="55"/>
       <c r="C25" s="56" t="s">
         <v>38</v>
@@ -3134,7 +3152,7 @@
       <c r="AI25" s="12"/>
     </row>
     <row r="26" spans="1:35" ht="30" customHeight="1">
-      <c r="A26" s="200"/>
+      <c r="A26" s="184"/>
       <c r="B26" s="13"/>
       <c r="C26" s="14" t="s">
         <v>39</v>
@@ -3181,12 +3199,12 @@
       <c r="AI26" s="12"/>
     </row>
     <row r="27" spans="1:35" ht="30" customHeight="1">
-      <c r="A27" s="200"/>
+      <c r="A27" s="184"/>
       <c r="B27" s="38"/>
-      <c r="C27" s="191" t="s">
+      <c r="C27" s="186" t="s">
         <v>25</v>
       </c>
-      <c r="D27" s="192"/>
+      <c r="D27" s="187"/>
       <c r="E27" s="39">
         <f>SUM(E19:E26)</f>
         <v>20</v>
@@ -3197,15 +3215,15 @@
         <v>58</v>
       </c>
       <c r="H27" s="62">
-        <f t="shared" ref="H27:J27" si="1">SUM(H19:H26)</f>
+        <f>SUM(H19:H26)</f>
         <v>236</v>
       </c>
       <c r="I27" s="62">
-        <f t="shared" si="1"/>
+        <f>SUM(I19:I26)</f>
         <v>8</v>
       </c>
       <c r="J27" s="62">
-        <f t="shared" si="1"/>
+        <f>SUM(J19:J26)</f>
         <v>91</v>
       </c>
       <c r="K27" s="41"/>
@@ -3346,11 +3364,11 @@
       <c r="AI30" s="3"/>
     </row>
     <row r="31" spans="1:35" ht="15.75">
-      <c r="A31" s="211" t="s">
+      <c r="A31" s="185" t="s">
         <v>41</v>
       </c>
       <c r="B31" s="68"/>
-      <c r="C31" s="195" t="s">
+      <c r="C31" s="201" t="s">
         <v>42</v>
       </c>
       <c r="D31" s="196"/>
@@ -3387,22 +3405,22 @@
       <c r="AI31" s="69"/>
     </row>
     <row r="32" spans="1:35" ht="15.75">
-      <c r="A32" s="200"/>
+      <c r="A32" s="184"/>
       <c r="B32" s="68"/>
-      <c r="C32" s="199" t="s">
+      <c r="C32" s="209" t="s">
         <v>43</v>
       </c>
-      <c r="D32" s="200"/>
-      <c r="E32" s="200"/>
-      <c r="F32" s="200"/>
-      <c r="G32" s="200"/>
-      <c r="H32" s="200"/>
-      <c r="I32" s="200"/>
-      <c r="J32" s="200"/>
-      <c r="K32" s="200"/>
-      <c r="L32" s="200"/>
-      <c r="M32" s="200"/>
-      <c r="N32" s="201"/>
+      <c r="D32" s="184"/>
+      <c r="E32" s="184"/>
+      <c r="F32" s="184"/>
+      <c r="G32" s="184"/>
+      <c r="H32" s="184"/>
+      <c r="I32" s="184"/>
+      <c r="J32" s="184"/>
+      <c r="K32" s="184"/>
+      <c r="L32" s="184"/>
+      <c r="M32" s="184"/>
+      <c r="N32" s="194"/>
       <c r="O32" s="69"/>
       <c r="P32" s="69"/>
       <c r="Q32" s="69"/>
@@ -3426,22 +3444,22 @@
       <c r="AI32" s="69"/>
     </row>
     <row r="33" spans="1:35" ht="15.75">
-      <c r="A33" s="200"/>
+      <c r="A33" s="184"/>
       <c r="B33" s="70"/>
-      <c r="C33" s="182" t="s">
+      <c r="C33" s="205" t="s">
         <v>27</v>
       </c>
-      <c r="D33" s="183"/>
-      <c r="E33" s="183"/>
-      <c r="F33" s="183"/>
-      <c r="G33" s="183"/>
-      <c r="H33" s="183"/>
-      <c r="I33" s="183"/>
-      <c r="J33" s="183"/>
-      <c r="K33" s="183"/>
-      <c r="L33" s="183"/>
-      <c r="M33" s="183"/>
-      <c r="N33" s="184"/>
+      <c r="D33" s="199"/>
+      <c r="E33" s="199"/>
+      <c r="F33" s="199"/>
+      <c r="G33" s="199"/>
+      <c r="H33" s="199"/>
+      <c r="I33" s="199"/>
+      <c r="J33" s="199"/>
+      <c r="K33" s="199"/>
+      <c r="L33" s="199"/>
+      <c r="M33" s="199"/>
+      <c r="N33" s="200"/>
       <c r="O33" s="69"/>
       <c r="P33" s="69"/>
       <c r="Q33" s="69"/>
@@ -3465,7 +3483,7 @@
       <c r="AI33" s="69"/>
     </row>
     <row r="34" spans="1:35" ht="30.75" customHeight="1">
-      <c r="A34" s="200"/>
+      <c r="A34" s="184"/>
       <c r="B34" s="5"/>
       <c r="C34" s="71" t="s">
         <v>4</v>
@@ -3516,7 +3534,7 @@
       <c r="AI34" s="12"/>
     </row>
     <row r="35" spans="1:35" ht="15.75">
-      <c r="A35" s="200"/>
+      <c r="A35" s="184"/>
       <c r="B35" s="77"/>
       <c r="C35" s="78" t="s">
         <v>45</v>
@@ -3564,7 +3582,7 @@
       <c r="AI35" s="3"/>
     </row>
     <row r="36" spans="1:35" ht="15.75">
-      <c r="A36" s="200"/>
+      <c r="A36" s="184"/>
       <c r="B36" s="77"/>
       <c r="C36" s="83" t="s">
         <v>46</v>
@@ -3572,7 +3590,7 @@
       <c r="D36" s="84" t="s">
         <v>47</v>
       </c>
-      <c r="E36" s="198">
+      <c r="E36" s="208">
         <v>9</v>
       </c>
       <c r="F36" s="81">
@@ -3613,13 +3631,13 @@
       <c r="AI36" s="3"/>
     </row>
     <row r="37" spans="1:35" ht="15.75">
-      <c r="A37" s="200"/>
+      <c r="A37" s="184"/>
       <c r="B37" s="77"/>
       <c r="C37" s="85"/>
       <c r="D37" s="84" t="s">
         <v>48</v>
       </c>
-      <c r="E37" s="209"/>
+      <c r="E37" s="219"/>
       <c r="F37" s="81">
         <v>3</v>
       </c>
@@ -3658,13 +3676,13 @@
       <c r="AI37" s="3"/>
     </row>
     <row r="38" spans="1:35" ht="15.75">
-      <c r="A38" s="200"/>
+      <c r="A38" s="184"/>
       <c r="B38" s="77"/>
       <c r="C38" s="86"/>
       <c r="D38" s="84" t="s">
         <v>49</v>
       </c>
-      <c r="E38" s="194"/>
+      <c r="E38" s="207"/>
       <c r="F38" s="81">
         <v>2</v>
       </c>
@@ -3703,7 +3721,7 @@
       <c r="AI38" s="3"/>
     </row>
     <row r="39" spans="1:35" ht="15.75">
-      <c r="A39" s="200"/>
+      <c r="A39" s="184"/>
       <c r="B39" s="77"/>
       <c r="C39" s="78" t="s">
         <v>50</v>
@@ -3752,9 +3770,9 @@
       <c r="AI39" s="3"/>
     </row>
     <row r="40" spans="1:35" ht="15.75">
-      <c r="A40" s="200"/>
+      <c r="A40" s="184"/>
       <c r="B40" s="77"/>
-      <c r="C40" s="207" t="s">
+      <c r="C40" s="190" t="s">
         <v>52</v>
       </c>
       <c r="D40" s="87" t="s">
@@ -3797,9 +3815,9 @@
       <c r="AI40" s="3"/>
     </row>
     <row r="41" spans="1:35" ht="15.75">
-      <c r="A41" s="200"/>
+      <c r="A41" s="184"/>
       <c r="B41" s="77"/>
-      <c r="C41" s="208"/>
+      <c r="C41" s="191"/>
       <c r="D41" s="88" t="s">
         <v>22</v>
       </c>
@@ -3840,12 +3858,12 @@
       <c r="AI41" s="3"/>
     </row>
     <row r="42" spans="1:35" ht="16.5" customHeight="1">
-      <c r="A42" s="200"/>
+      <c r="A42" s="184"/>
       <c r="B42" s="38"/>
-      <c r="C42" s="205" t="s">
+      <c r="C42" s="217" t="s">
         <v>25</v>
       </c>
-      <c r="D42" s="206"/>
+      <c r="D42" s="218"/>
       <c r="E42" s="95">
         <f>SUM(E35:E41)</f>
         <v>21</v>
@@ -3856,15 +3874,15 @@
         <v>90</v>
       </c>
       <c r="H42" s="97">
-        <f t="shared" ref="H42:J42" si="2">SUM(H35:H41)</f>
+        <f t="shared" ref="H42:J42" si="0">SUM(H35:H41)</f>
         <v>72</v>
       </c>
       <c r="I42" s="97">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>102</v>
       </c>
       <c r="J42" s="97">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="K42" s="98"/>
@@ -3894,7 +3912,7 @@
       <c r="AI42" s="12"/>
     </row>
     <row r="43" spans="1:35" ht="15.75">
-      <c r="A43" s="200"/>
+      <c r="A43" s="184"/>
       <c r="B43" s="77"/>
       <c r="C43" s="77"/>
       <c r="D43" s="63"/>
@@ -3931,9 +3949,9 @@
       <c r="AI43" s="3"/>
     </row>
     <row r="44" spans="1:35" ht="15.75">
-      <c r="A44" s="200"/>
+      <c r="A44" s="184"/>
       <c r="B44" s="68"/>
-      <c r="C44" s="195" t="s">
+      <c r="C44" s="201" t="s">
         <v>43</v>
       </c>
       <c r="D44" s="196"/>
@@ -3970,22 +3988,22 @@
       <c r="AI44" s="69"/>
     </row>
     <row r="45" spans="1:35" ht="15.75">
-      <c r="A45" s="200"/>
+      <c r="A45" s="184"/>
       <c r="B45" s="101"/>
-      <c r="C45" s="182" t="s">
+      <c r="C45" s="205" t="s">
         <v>53</v>
       </c>
-      <c r="D45" s="183"/>
-      <c r="E45" s="183"/>
-      <c r="F45" s="183"/>
-      <c r="G45" s="183"/>
-      <c r="H45" s="183"/>
-      <c r="I45" s="183"/>
-      <c r="J45" s="183"/>
-      <c r="K45" s="183"/>
-      <c r="L45" s="183"/>
-      <c r="M45" s="183"/>
-      <c r="N45" s="184"/>
+      <c r="D45" s="199"/>
+      <c r="E45" s="199"/>
+      <c r="F45" s="199"/>
+      <c r="G45" s="199"/>
+      <c r="H45" s="199"/>
+      <c r="I45" s="199"/>
+      <c r="J45" s="199"/>
+      <c r="K45" s="199"/>
+      <c r="L45" s="199"/>
+      <c r="M45" s="199"/>
+      <c r="N45" s="200"/>
       <c r="O45" s="69"/>
       <c r="P45" s="69"/>
       <c r="Q45" s="69"/>
@@ -4009,22 +4027,22 @@
       <c r="AI45" s="69"/>
     </row>
     <row r="46" spans="1:35" ht="15.75">
-      <c r="A46" s="200"/>
+      <c r="A46" s="184"/>
       <c r="B46" s="102"/>
-      <c r="C46" s="218" t="s">
+      <c r="C46" s="202" t="s">
         <v>54</v>
       </c>
-      <c r="D46" s="219"/>
-      <c r="E46" s="219"/>
-      <c r="F46" s="219"/>
-      <c r="G46" s="219"/>
-      <c r="H46" s="219"/>
-      <c r="I46" s="219"/>
-      <c r="J46" s="219"/>
-      <c r="K46" s="219"/>
-      <c r="L46" s="219"/>
-      <c r="M46" s="219"/>
-      <c r="N46" s="220"/>
+      <c r="D46" s="203"/>
+      <c r="E46" s="203"/>
+      <c r="F46" s="203"/>
+      <c r="G46" s="203"/>
+      <c r="H46" s="203"/>
+      <c r="I46" s="203"/>
+      <c r="J46" s="203"/>
+      <c r="K46" s="203"/>
+      <c r="L46" s="203"/>
+      <c r="M46" s="203"/>
+      <c r="N46" s="204"/>
       <c r="O46" s="3"/>
       <c r="P46" s="3"/>
       <c r="Q46" s="3"/>
@@ -4048,7 +4066,7 @@
       <c r="AI46" s="3"/>
     </row>
     <row r="47" spans="1:35" ht="15.75">
-      <c r="A47" s="200"/>
+      <c r="A47" s="184"/>
       <c r="B47" s="77"/>
       <c r="C47" s="103" t="s">
         <v>55</v>
@@ -4097,7 +4115,7 @@
       <c r="AI47" s="3"/>
     </row>
     <row r="48" spans="1:35" ht="15.75">
-      <c r="A48" s="200"/>
+      <c r="A48" s="184"/>
       <c r="B48" s="77"/>
       <c r="C48" s="110" t="s">
         <v>57</v>
@@ -4146,7 +4164,7 @@
       <c r="AI48" s="3"/>
     </row>
     <row r="49" spans="1:35" ht="15.75">
-      <c r="A49" s="200"/>
+      <c r="A49" s="184"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
       <c r="D49" s="63"/>
@@ -4183,22 +4201,22 @@
       <c r="AI49" s="3"/>
     </row>
     <row r="50" spans="1:35" ht="15.75">
-      <c r="A50" s="200"/>
+      <c r="A50" s="184"/>
       <c r="B50" s="102"/>
-      <c r="C50" s="189" t="s">
+      <c r="C50" s="216" t="s">
         <v>59</v>
       </c>
-      <c r="D50" s="186"/>
-      <c r="E50" s="186"/>
-      <c r="F50" s="186"/>
-      <c r="G50" s="186"/>
-      <c r="H50" s="186"/>
-      <c r="I50" s="186"/>
-      <c r="J50" s="186"/>
-      <c r="K50" s="186"/>
-      <c r="L50" s="186"/>
-      <c r="M50" s="186"/>
-      <c r="N50" s="187"/>
+      <c r="D50" s="211"/>
+      <c r="E50" s="211"/>
+      <c r="F50" s="211"/>
+      <c r="G50" s="211"/>
+      <c r="H50" s="211"/>
+      <c r="I50" s="211"/>
+      <c r="J50" s="211"/>
+      <c r="K50" s="211"/>
+      <c r="L50" s="211"/>
+      <c r="M50" s="211"/>
+      <c r="N50" s="212"/>
       <c r="O50" s="3"/>
       <c r="P50" s="3"/>
       <c r="Q50" s="3"/>
@@ -4222,7 +4240,7 @@
       <c r="AI50" s="3"/>
     </row>
     <row r="51" spans="1:35" ht="15.75">
-      <c r="A51" s="200"/>
+      <c r="A51" s="184"/>
       <c r="B51" s="77"/>
       <c r="C51" s="117" t="s">
         <v>60</v>
@@ -4272,7 +4290,7 @@
       <c r="AI51" s="3"/>
     </row>
     <row r="52" spans="1:35" ht="15.75">
-      <c r="A52" s="200"/>
+      <c r="A52" s="184"/>
       <c r="B52" s="77"/>
       <c r="C52" s="117" t="s">
         <v>61</v>
@@ -4320,7 +4338,7 @@
       <c r="AI52" s="3"/>
     </row>
     <row r="53" spans="1:35" ht="15.75">
-      <c r="A53" s="200"/>
+      <c r="A53" s="184"/>
       <c r="B53" s="3"/>
       <c r="C53" s="125"/>
       <c r="D53" s="63"/>
@@ -4357,22 +4375,22 @@
       <c r="AI53" s="3"/>
     </row>
     <row r="54" spans="1:35" ht="15.75">
-      <c r="A54" s="200"/>
+      <c r="A54" s="184"/>
       <c r="B54" s="102"/>
-      <c r="C54" s="202" t="s">
+      <c r="C54" s="213" t="s">
         <v>62</v>
       </c>
-      <c r="D54" s="203"/>
-      <c r="E54" s="203"/>
-      <c r="F54" s="203"/>
-      <c r="G54" s="203"/>
-      <c r="H54" s="203"/>
-      <c r="I54" s="203"/>
-      <c r="J54" s="203"/>
-      <c r="K54" s="203"/>
-      <c r="L54" s="203"/>
-      <c r="M54" s="203"/>
-      <c r="N54" s="204"/>
+      <c r="D54" s="214"/>
+      <c r="E54" s="214"/>
+      <c r="F54" s="214"/>
+      <c r="G54" s="214"/>
+      <c r="H54" s="214"/>
+      <c r="I54" s="214"/>
+      <c r="J54" s="214"/>
+      <c r="K54" s="214"/>
+      <c r="L54" s="214"/>
+      <c r="M54" s="214"/>
+      <c r="N54" s="215"/>
       <c r="O54" s="3"/>
       <c r="P54" s="3"/>
       <c r="Q54" s="3"/>
@@ -4396,7 +4414,7 @@
       <c r="AI54" s="3"/>
     </row>
     <row r="55" spans="1:35" ht="15.75">
-      <c r="A55" s="200"/>
+      <c r="A55" s="184"/>
       <c r="B55" s="77"/>
       <c r="C55" s="127" t="s">
         <v>63</v>
@@ -4445,7 +4463,7 @@
       <c r="AI55" s="3"/>
     </row>
     <row r="56" spans="1:35" ht="31.5">
-      <c r="A56" s="200"/>
+      <c r="A56" s="184"/>
       <c r="B56" s="77"/>
       <c r="C56" s="134" t="s">
         <v>64</v>
@@ -4490,7 +4508,7 @@
       <c r="AI56" s="3"/>
     </row>
     <row r="57" spans="1:35" ht="15.75">
-      <c r="A57" s="200"/>
+      <c r="A57" s="184"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
       <c r="D57" s="63"/>
@@ -4527,22 +4545,22 @@
       <c r="AI57" s="3"/>
     </row>
     <row r="58" spans="1:35" ht="15.75">
-      <c r="A58" s="200"/>
+      <c r="A58" s="184"/>
       <c r="B58" s="102"/>
-      <c r="C58" s="190" t="s">
+      <c r="C58" s="210" t="s">
         <v>66</v>
       </c>
-      <c r="D58" s="186"/>
-      <c r="E58" s="186"/>
-      <c r="F58" s="186"/>
-      <c r="G58" s="186"/>
-      <c r="H58" s="186"/>
-      <c r="I58" s="186"/>
-      <c r="J58" s="186"/>
-      <c r="K58" s="186"/>
-      <c r="L58" s="186"/>
-      <c r="M58" s="186"/>
-      <c r="N58" s="187"/>
+      <c r="D58" s="211"/>
+      <c r="E58" s="211"/>
+      <c r="F58" s="211"/>
+      <c r="G58" s="211"/>
+      <c r="H58" s="211"/>
+      <c r="I58" s="211"/>
+      <c r="J58" s="211"/>
+      <c r="K58" s="211"/>
+      <c r="L58" s="211"/>
+      <c r="M58" s="211"/>
+      <c r="N58" s="212"/>
       <c r="O58" s="3"/>
       <c r="P58" s="3"/>
       <c r="Q58" s="3"/>
@@ -4566,7 +4584,7 @@
       <c r="AI58" s="3"/>
     </row>
     <row r="59" spans="1:35" ht="15.75">
-      <c r="A59" s="200"/>
+      <c r="A59" s="184"/>
       <c r="B59" s="77"/>
       <c r="C59" s="103" t="s">
         <v>67</v>
@@ -4615,7 +4633,7 @@
       <c r="AI59" s="3"/>
     </row>
     <row r="60" spans="1:35" ht="15.75">
-      <c r="A60" s="200"/>
+      <c r="A60" s="184"/>
       <c r="B60" s="77"/>
       <c r="C60" s="141" t="s">
         <v>68</v>
@@ -4664,7 +4682,7 @@
       <c r="AI60" s="3"/>
     </row>
     <row r="61" spans="1:35" ht="15.75">
-      <c r="A61" s="200"/>
+      <c r="A61" s="184"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
       <c r="D61" s="63"/>
@@ -4701,7 +4719,7 @@
       <c r="AI61" s="3"/>
     </row>
     <row r="62" spans="1:35" ht="5.25" customHeight="1">
-      <c r="A62" s="200"/>
+      <c r="A62" s="184"/>
       <c r="B62" s="148"/>
       <c r="C62" s="149"/>
       <c r="D62" s="150"/>
@@ -4738,7 +4756,7 @@
       <c r="AI62" s="151"/>
     </row>
     <row r="63" spans="1:35" ht="15.75">
-      <c r="A63" s="200"/>
+      <c r="A63" s="184"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
       <c r="D63" s="63"/>
@@ -4775,9 +4793,9 @@
       <c r="AI63" s="3"/>
     </row>
     <row r="64" spans="1:35" ht="15.75">
-      <c r="A64" s="200"/>
+      <c r="A64" s="184"/>
       <c r="B64" s="68"/>
-      <c r="C64" s="195" t="s">
+      <c r="C64" s="201" t="s">
         <v>42</v>
       </c>
       <c r="D64" s="196"/>
@@ -4814,22 +4832,22 @@
       <c r="AI64" s="69"/>
     </row>
     <row r="65" spans="1:35" ht="15.75">
-      <c r="A65" s="200"/>
+      <c r="A65" s="184"/>
       <c r="B65" s="68"/>
-      <c r="C65" s="199" t="s">
+      <c r="C65" s="209" t="s">
         <v>70</v>
       </c>
-      <c r="D65" s="200"/>
-      <c r="E65" s="200"/>
-      <c r="F65" s="200"/>
-      <c r="G65" s="200"/>
-      <c r="H65" s="200"/>
-      <c r="I65" s="200"/>
-      <c r="J65" s="200"/>
-      <c r="K65" s="200"/>
-      <c r="L65" s="200"/>
-      <c r="M65" s="200"/>
-      <c r="N65" s="201"/>
+      <c r="D65" s="184"/>
+      <c r="E65" s="184"/>
+      <c r="F65" s="184"/>
+      <c r="G65" s="184"/>
+      <c r="H65" s="184"/>
+      <c r="I65" s="184"/>
+      <c r="J65" s="184"/>
+      <c r="K65" s="184"/>
+      <c r="L65" s="184"/>
+      <c r="M65" s="184"/>
+      <c r="N65" s="194"/>
       <c r="O65" s="69"/>
       <c r="P65" s="69"/>
       <c r="Q65" s="69"/>
@@ -4853,22 +4871,22 @@
       <c r="AI65" s="69"/>
     </row>
     <row r="66" spans="1:35" ht="15.75">
-      <c r="A66" s="200"/>
+      <c r="A66" s="184"/>
       <c r="B66" s="70"/>
-      <c r="C66" s="182" t="s">
+      <c r="C66" s="205" t="s">
         <v>27</v>
       </c>
-      <c r="D66" s="183"/>
-      <c r="E66" s="183"/>
-      <c r="F66" s="183"/>
-      <c r="G66" s="183"/>
-      <c r="H66" s="183"/>
-      <c r="I66" s="183"/>
-      <c r="J66" s="183"/>
-      <c r="K66" s="183"/>
-      <c r="L66" s="183"/>
-      <c r="M66" s="183"/>
-      <c r="N66" s="184"/>
+      <c r="D66" s="199"/>
+      <c r="E66" s="199"/>
+      <c r="F66" s="199"/>
+      <c r="G66" s="199"/>
+      <c r="H66" s="199"/>
+      <c r="I66" s="199"/>
+      <c r="J66" s="199"/>
+      <c r="K66" s="199"/>
+      <c r="L66" s="199"/>
+      <c r="M66" s="199"/>
+      <c r="N66" s="200"/>
       <c r="O66" s="69"/>
       <c r="P66" s="69"/>
       <c r="Q66" s="69"/>
@@ -4892,7 +4910,7 @@
       <c r="AI66" s="69"/>
     </row>
     <row r="67" spans="1:35" ht="30.75" customHeight="1">
-      <c r="A67" s="200"/>
+      <c r="A67" s="184"/>
       <c r="B67" s="5"/>
       <c r="C67" s="6" t="s">
         <v>4</v>
@@ -4945,7 +4963,7 @@
       <c r="AI67" s="12"/>
     </row>
     <row r="68" spans="1:35" ht="15.75">
-      <c r="A68" s="200"/>
+      <c r="A68" s="184"/>
       <c r="B68" s="77"/>
       <c r="C68" s="78" t="s">
         <v>72</v>
@@ -4992,7 +5010,7 @@
       <c r="AI68" s="3"/>
     </row>
     <row r="69" spans="1:35" ht="27.75" customHeight="1">
-      <c r="A69" s="200"/>
+      <c r="A69" s="184"/>
       <c r="B69" s="77"/>
       <c r="C69" s="78" t="s">
         <v>74</v>
@@ -5039,7 +5057,7 @@
       <c r="AI69" s="3"/>
     </row>
     <row r="70" spans="1:35" ht="15.75">
-      <c r="A70" s="200"/>
+      <c r="A70" s="184"/>
       <c r="B70" s="77"/>
       <c r="C70" s="78" t="s">
         <v>76</v>
@@ -5088,15 +5106,15 @@
       <c r="AI70" s="3"/>
     </row>
     <row r="71" spans="1:35" ht="15.75">
-      <c r="A71" s="200"/>
+      <c r="A71" s="184"/>
       <c r="B71" s="77"/>
-      <c r="C71" s="207" t="s">
+      <c r="C71" s="190" t="s">
         <v>78</v>
       </c>
       <c r="D71" s="156" t="s">
         <v>79</v>
       </c>
-      <c r="E71" s="198">
+      <c r="E71" s="208">
         <v>3</v>
       </c>
       <c r="F71" s="81">
@@ -5137,13 +5155,13 @@
       <c r="AI71" s="3"/>
     </row>
     <row r="72" spans="1:35" ht="15.75">
-      <c r="A72" s="200"/>
+      <c r="A72" s="184"/>
       <c r="B72" s="77"/>
-      <c r="C72" s="208"/>
+      <c r="C72" s="191"/>
       <c r="D72" s="156" t="s">
         <v>22</v>
       </c>
-      <c r="E72" s="194"/>
+      <c r="E72" s="207"/>
       <c r="F72" s="81">
         <v>1.5</v>
       </c>
@@ -5182,7 +5200,7 @@
       <c r="AI72" s="3"/>
     </row>
     <row r="73" spans="1:35" ht="15.75">
-      <c r="A73" s="200"/>
+      <c r="A73" s="184"/>
       <c r="B73" s="77"/>
       <c r="C73" s="78" t="s">
         <v>80</v>
@@ -5231,12 +5249,12 @@
       <c r="AI73" s="3"/>
     </row>
     <row r="74" spans="1:35" ht="15.75">
-      <c r="A74" s="200"/>
+      <c r="A74" s="184"/>
       <c r="B74" s="38"/>
-      <c r="C74" s="212" t="s">
+      <c r="C74" s="188" t="s">
         <v>25</v>
       </c>
-      <c r="D74" s="213"/>
+      <c r="D74" s="189"/>
       <c r="E74" s="95">
         <f>SUM(E68:E73)</f>
         <v>21</v>
@@ -5247,15 +5265,15 @@
         <v>84</v>
       </c>
       <c r="H74" s="96">
-        <f t="shared" ref="H74:J74" si="3">SUM(H68:H73)</f>
+        <f t="shared" ref="H74:J74" si="1">SUM(H68:H73)</f>
         <v>78</v>
       </c>
       <c r="I74" s="96">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>90</v>
       </c>
       <c r="J74" s="96">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>90</v>
       </c>
       <c r="K74" s="163"/>
@@ -5285,7 +5303,7 @@
       <c r="AI74" s="3"/>
     </row>
     <row r="75" spans="1:35" ht="15.75">
-      <c r="A75" s="200"/>
+      <c r="A75" s="184"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
       <c r="D75" s="63"/>
@@ -5322,9 +5340,9 @@
       <c r="AI75" s="3"/>
     </row>
     <row r="76" spans="1:35" ht="15.75">
-      <c r="A76" s="200"/>
+      <c r="A76" s="184"/>
       <c r="B76" s="68"/>
-      <c r="C76" s="195" t="s">
+      <c r="C76" s="201" t="s">
         <v>70</v>
       </c>
       <c r="D76" s="196"/>
@@ -5361,22 +5379,22 @@
       <c r="AI76" s="69"/>
     </row>
     <row r="77" spans="1:35" ht="15.75">
-      <c r="A77" s="200"/>
+      <c r="A77" s="184"/>
       <c r="B77" s="101"/>
-      <c r="C77" s="182" t="s">
+      <c r="C77" s="205" t="s">
         <v>53</v>
       </c>
-      <c r="D77" s="183"/>
-      <c r="E77" s="183"/>
-      <c r="F77" s="183"/>
-      <c r="G77" s="183"/>
-      <c r="H77" s="183"/>
-      <c r="I77" s="183"/>
-      <c r="J77" s="183"/>
-      <c r="K77" s="183"/>
-      <c r="L77" s="183"/>
-      <c r="M77" s="183"/>
-      <c r="N77" s="184"/>
+      <c r="D77" s="199"/>
+      <c r="E77" s="199"/>
+      <c r="F77" s="199"/>
+      <c r="G77" s="199"/>
+      <c r="H77" s="199"/>
+      <c r="I77" s="199"/>
+      <c r="J77" s="199"/>
+      <c r="K77" s="199"/>
+      <c r="L77" s="199"/>
+      <c r="M77" s="199"/>
+      <c r="N77" s="200"/>
       <c r="O77" s="69"/>
       <c r="P77" s="69"/>
       <c r="Q77" s="69"/>
@@ -5400,22 +5418,22 @@
       <c r="AI77" s="69"/>
     </row>
     <row r="78" spans="1:35" ht="15.75">
-      <c r="A78" s="200"/>
+      <c r="A78" s="184"/>
       <c r="B78" s="102"/>
-      <c r="C78" s="188" t="s">
+      <c r="C78" s="221" t="s">
         <v>54</v>
       </c>
-      <c r="D78" s="186"/>
-      <c r="E78" s="186"/>
-      <c r="F78" s="186"/>
-      <c r="G78" s="186"/>
-      <c r="H78" s="186"/>
-      <c r="I78" s="186"/>
-      <c r="J78" s="186"/>
-      <c r="K78" s="186"/>
-      <c r="L78" s="186"/>
-      <c r="M78" s="186"/>
-      <c r="N78" s="187"/>
+      <c r="D78" s="211"/>
+      <c r="E78" s="211"/>
+      <c r="F78" s="211"/>
+      <c r="G78" s="211"/>
+      <c r="H78" s="211"/>
+      <c r="I78" s="211"/>
+      <c r="J78" s="211"/>
+      <c r="K78" s="211"/>
+      <c r="L78" s="211"/>
+      <c r="M78" s="211"/>
+      <c r="N78" s="212"/>
       <c r="O78" s="3"/>
       <c r="P78" s="3"/>
       <c r="Q78" s="3"/>
@@ -5439,7 +5457,7 @@
       <c r="AI78" s="3"/>
     </row>
     <row r="79" spans="1:35" ht="15.75">
-      <c r="A79" s="200"/>
+      <c r="A79" s="184"/>
       <c r="B79" s="77"/>
       <c r="C79" s="103" t="s">
         <v>82</v>
@@ -5488,7 +5506,7 @@
       <c r="AI79" s="3"/>
     </row>
     <row r="80" spans="1:35" ht="15.75">
-      <c r="A80" s="200"/>
+      <c r="A80" s="184"/>
       <c r="B80" s="77"/>
       <c r="C80" s="110" t="s">
         <v>84</v>
@@ -5537,7 +5555,7 @@
       <c r="AI80" s="3"/>
     </row>
     <row r="81" spans="1:35" ht="15.75">
-      <c r="A81" s="200"/>
+      <c r="A81" s="184"/>
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
       <c r="D81" s="63"/>
@@ -5574,22 +5592,22 @@
       <c r="AI81" s="3"/>
     </row>
     <row r="82" spans="1:35" ht="15.75">
-      <c r="A82" s="200"/>
+      <c r="A82" s="184"/>
       <c r="B82" s="102"/>
-      <c r="C82" s="189" t="s">
+      <c r="C82" s="216" t="s">
         <v>59</v>
       </c>
-      <c r="D82" s="186"/>
-      <c r="E82" s="186"/>
-      <c r="F82" s="186"/>
-      <c r="G82" s="186"/>
-      <c r="H82" s="186"/>
-      <c r="I82" s="186"/>
-      <c r="J82" s="186"/>
-      <c r="K82" s="186"/>
-      <c r="L82" s="186"/>
-      <c r="M82" s="186"/>
-      <c r="N82" s="187"/>
+      <c r="D82" s="211"/>
+      <c r="E82" s="211"/>
+      <c r="F82" s="211"/>
+      <c r="G82" s="211"/>
+      <c r="H82" s="211"/>
+      <c r="I82" s="211"/>
+      <c r="J82" s="211"/>
+      <c r="K82" s="211"/>
+      <c r="L82" s="211"/>
+      <c r="M82" s="211"/>
+      <c r="N82" s="212"/>
       <c r="O82" s="3"/>
       <c r="P82" s="3"/>
       <c r="Q82" s="3"/>
@@ -5613,7 +5631,7 @@
       <c r="AI82" s="3"/>
     </row>
     <row r="83" spans="1:35" ht="15.75">
-      <c r="A83" s="200"/>
+      <c r="A83" s="184"/>
       <c r="B83" s="77"/>
       <c r="C83" s="117" t="s">
         <v>86</v>
@@ -5662,7 +5680,7 @@
       <c r="AI83" s="3"/>
     </row>
     <row r="84" spans="1:35" ht="15.75">
-      <c r="A84" s="200"/>
+      <c r="A84" s="184"/>
       <c r="B84" s="77"/>
       <c r="C84" s="169" t="s">
         <v>88</v>
@@ -5711,7 +5729,7 @@
       <c r="AI84" s="3"/>
     </row>
     <row r="85" spans="1:35" ht="15.75">
-      <c r="A85" s="200"/>
+      <c r="A85" s="184"/>
       <c r="B85" s="3"/>
       <c r="C85" s="3"/>
       <c r="D85" s="63"/>
@@ -5748,22 +5766,22 @@
       <c r="AI85" s="3"/>
     </row>
     <row r="86" spans="1:35" ht="15.75">
-      <c r="A86" s="200"/>
+      <c r="A86" s="184"/>
       <c r="B86" s="102"/>
-      <c r="C86" s="185" t="s">
+      <c r="C86" s="220" t="s">
         <v>62</v>
       </c>
-      <c r="D86" s="186"/>
-      <c r="E86" s="186"/>
-      <c r="F86" s="186"/>
-      <c r="G86" s="186"/>
-      <c r="H86" s="186"/>
-      <c r="I86" s="186"/>
-      <c r="J86" s="186"/>
-      <c r="K86" s="186"/>
-      <c r="L86" s="186"/>
-      <c r="M86" s="186"/>
-      <c r="N86" s="187"/>
+      <c r="D86" s="211"/>
+      <c r="E86" s="211"/>
+      <c r="F86" s="211"/>
+      <c r="G86" s="211"/>
+      <c r="H86" s="211"/>
+      <c r="I86" s="211"/>
+      <c r="J86" s="211"/>
+      <c r="K86" s="211"/>
+      <c r="L86" s="211"/>
+      <c r="M86" s="211"/>
+      <c r="N86" s="212"/>
       <c r="O86" s="3"/>
       <c r="P86" s="3"/>
       <c r="Q86" s="3"/>
@@ -5787,7 +5805,7 @@
       <c r="AI86" s="3"/>
     </row>
     <row r="87" spans="1:35" ht="15.75">
-      <c r="A87" s="200"/>
+      <c r="A87" s="184"/>
       <c r="B87" s="77"/>
       <c r="C87" s="103" t="s">
         <v>90</v>
@@ -5836,7 +5854,7 @@
       <c r="AI87" s="3"/>
     </row>
     <row r="88" spans="1:35" ht="15.75">
-      <c r="A88" s="200"/>
+      <c r="A88" s="184"/>
       <c r="B88" s="77"/>
       <c r="C88" s="134" t="s">
         <v>91</v>
@@ -5881,7 +5899,7 @@
       <c r="AI88" s="3"/>
     </row>
     <row r="89" spans="1:35" ht="15.75">
-      <c r="A89" s="200"/>
+      <c r="A89" s="184"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
       <c r="D89" s="63"/>
@@ -5918,22 +5936,22 @@
       <c r="AI89" s="3"/>
     </row>
     <row r="90" spans="1:35" ht="15.75">
-      <c r="A90" s="200"/>
+      <c r="A90" s="184"/>
       <c r="B90" s="102"/>
-      <c r="C90" s="190" t="s">
+      <c r="C90" s="210" t="s">
         <v>66</v>
       </c>
-      <c r="D90" s="186"/>
-      <c r="E90" s="186"/>
-      <c r="F90" s="186"/>
-      <c r="G90" s="186"/>
-      <c r="H90" s="186"/>
-      <c r="I90" s="186"/>
-      <c r="J90" s="186"/>
-      <c r="K90" s="186"/>
-      <c r="L90" s="186"/>
-      <c r="M90" s="186"/>
-      <c r="N90" s="187"/>
+      <c r="D90" s="211"/>
+      <c r="E90" s="211"/>
+      <c r="F90" s="211"/>
+      <c r="G90" s="211"/>
+      <c r="H90" s="211"/>
+      <c r="I90" s="211"/>
+      <c r="J90" s="211"/>
+      <c r="K90" s="211"/>
+      <c r="L90" s="211"/>
+      <c r="M90" s="211"/>
+      <c r="N90" s="212"/>
       <c r="O90" s="3"/>
       <c r="P90" s="3"/>
       <c r="Q90" s="3"/>
@@ -5957,7 +5975,7 @@
       <c r="AI90" s="3"/>
     </row>
     <row r="91" spans="1:35" ht="15.75">
-      <c r="A91" s="200"/>
+      <c r="A91" s="184"/>
       <c r="B91" s="77"/>
       <c r="C91" s="103" t="s">
         <v>93</v>
@@ -6006,7 +6024,7 @@
       <c r="AI91" s="3"/>
     </row>
     <row r="92" spans="1:35" ht="15.75">
-      <c r="A92" s="200"/>
+      <c r="A92" s="184"/>
       <c r="B92" s="77"/>
       <c r="C92" s="141" t="s">
         <v>94</v>
@@ -40169,6 +40187,26 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="C77:N77"/>
+    <mergeCell ref="C86:N86"/>
+    <mergeCell ref="C78:N78"/>
+    <mergeCell ref="C82:N82"/>
+    <mergeCell ref="C90:N90"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="C76:N76"/>
+    <mergeCell ref="E71:E72"/>
+    <mergeCell ref="C65:N65"/>
+    <mergeCell ref="C66:N66"/>
+    <mergeCell ref="C64:N64"/>
+    <mergeCell ref="C58:N58"/>
+    <mergeCell ref="C54:N54"/>
+    <mergeCell ref="C50:N50"/>
+    <mergeCell ref="C32:N32"/>
+    <mergeCell ref="C31:N31"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="E36:E38"/>
     <mergeCell ref="A2:A27"/>
     <mergeCell ref="A31:A92"/>
     <mergeCell ref="C13:D13"/>
@@ -40185,26 +40223,6 @@
     <mergeCell ref="C46:N46"/>
     <mergeCell ref="C45:N45"/>
     <mergeCell ref="C33:N33"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="C76:N76"/>
-    <mergeCell ref="E71:E72"/>
-    <mergeCell ref="C65:N65"/>
-    <mergeCell ref="C66:N66"/>
-    <mergeCell ref="C64:N64"/>
-    <mergeCell ref="C58:N58"/>
-    <mergeCell ref="C54:N54"/>
-    <mergeCell ref="C50:N50"/>
-    <mergeCell ref="C32:N32"/>
-    <mergeCell ref="C31:N31"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="E36:E38"/>
-    <mergeCell ref="C77:N77"/>
-    <mergeCell ref="C86:N86"/>
-    <mergeCell ref="C78:N78"/>
-    <mergeCell ref="C82:N82"/>
-    <mergeCell ref="C90:N90"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -40215,10 +40233,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E968BCBF-36A6-464F-AF2B-64F7AA070C0D}">
   <sheetPr codeName="Feuil2"/>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -40248,17 +40266,19 @@
         <v>104</v>
       </c>
       <c r="B2" s="180">
-        <f>SUM('-R- List of courses'!G19,'-R- List of courses'!G20)</f>
+        <f>SUM('-R- List of courses'!G6,'-R- List of courses'!G19,'-R- List of courses'!G20)</f>
         <v>20</v>
       </c>
       <c r="C2" s="180">
         <f>SUM('-R- List of courses'!H6,'-R- List of courses'!H19,'-R- List of courses'!H20)</f>
         <v>106</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="180">
+        <f>SUM('-R- List of courses'!I6,'-R- List of courses'!I19,'-R- List of courses'!I20)</f>
         <v>0</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="180">
+        <f>SUM('-R- List of courses'!J6,'-R- List of courses'!J19,'-R- List of courses'!J20)</f>
         <v>0</v>
       </c>
     </row>
@@ -40267,18 +40287,19 @@
         <v>103</v>
       </c>
       <c r="B3" s="180">
-        <f>SUM('-R- List of courses'!G21)</f>
+        <f>SUM('-R- List of courses'!G7,'-R- List of courses'!G21)</f>
         <v>14</v>
       </c>
       <c r="C3" s="180">
         <f>SUM('-R- List of courses'!H7,'-R- List of courses'!H21)</f>
         <v>70</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="180">
+        <f>SUM('-R- List of courses'!I7,'-R- List of courses'!I21)</f>
         <v>0</v>
       </c>
       <c r="E3" s="180">
-        <f>SUM('-R- List of courses'!J21)</f>
+        <f>SUM('-R- List of courses'!J7,'-R- List of courses'!J21)</f>
         <v>21</v>
       </c>
     </row>
@@ -40287,18 +40308,19 @@
         <v>102</v>
       </c>
       <c r="B4" s="180">
-        <f>SUM('-R- List of courses'!G22)</f>
+        <f>SUM('-R- List of courses'!G9,'-R- List of courses'!G22)</f>
         <v>10</v>
       </c>
       <c r="C4" s="180">
         <f>SUM('-R- List of courses'!H9,'-R- List of courses'!H22)</f>
         <v>88</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="180">
+        <f>SUM('-R- List of courses'!I9,'-R- List of courses'!I22)</f>
         <v>0</v>
       </c>
       <c r="E4" s="180">
-        <f>SUM('-R- List of courses'!J22)</f>
+        <f>SUM('-R- List of courses'!J9,'-R- List of courses'!J22)</f>
         <v>21</v>
       </c>
     </row>
@@ -40306,17 +40328,20 @@
       <c r="A5" s="181" t="s">
         <v>101</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="180">
+        <f>SUM('-R- List of courses'!G10,'-R- List of courses'!G24)</f>
         <v>0</v>
       </c>
       <c r="C5" s="180">
-        <f>SUM('-R- List of courses'!H24,'-R- List of courses'!H10)</f>
+        <f>SUM('-R- List of courses'!H10,'-R- List of courses'!H24)</f>
         <v>84</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="180">
+        <f>SUM('-R- List of courses'!I10,'-R- List of courses'!I24)</f>
         <v>0</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="180">
+        <f>SUM('-R- List of courses'!J10,'-R- List of courses'!J24)</f>
         <v>42</v>
       </c>
     </row>
@@ -40324,17 +40349,20 @@
       <c r="A6" s="181" t="s">
         <v>100</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="180">
+        <f>SUM('-R- List of courses'!G11,'-R- List of courses'!G25)</f>
         <v>0</v>
       </c>
       <c r="C6" s="180">
         <f>SUM('-R- List of courses'!H11,'-R- List of courses'!H25)</f>
         <v>112</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="180">
+        <f>SUM('-R- List of courses'!I11,'-R- List of courses'!I25)</f>
         <v>0</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="180">
+        <f>SUM('-R- List of courses'!J11,'-R- List of courses'!J25)</f>
         <v>42</v>
       </c>
     </row>
@@ -40342,7 +40370,8 @@
       <c r="A7" s="181" t="s">
         <v>99</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="180">
+        <f>SUM('-R- List of courses'!G8,'-R- List of courses'!G23)</f>
         <v>14</v>
       </c>
       <c r="C7" s="180">
@@ -40350,7 +40379,7 @@
         <v>70</v>
       </c>
       <c r="D7" s="180">
-        <f>SUM('-R- List of courses'!I8,'-R- List of courses'!I22)</f>
+        <f>SUM('-R- List of courses'!I8,'-R- List of courses'!I23)</f>
         <v>0</v>
       </c>
       <c r="E7" s="180">
@@ -40366,10 +40395,12 @@
         <f>SUM('-R- List of courses'!G12,'-R- List of courses'!G26)</f>
         <v>0</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="180">
+        <f>SUM('-R- List of courses'!H12,'-R- List of courses'!H26)</f>
         <v>0</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="180">
+        <f>SUM('-R- List of courses'!I12,'-R- List of courses'!I26)</f>
         <v>8</v>
       </c>
       <c r="E8" s="180">
@@ -40378,81 +40409,837 @@
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="181" t="s">
+      <c r="A11" s="181"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="181"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="181"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="181"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="181"/>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="181"/>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="181"/>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="181"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D88A8C4-4B65-49EC-994F-DF8CED55AAB1}">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="182" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="182" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="182" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="182" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="182" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="181" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="180">
+        <f>SUM('-R- List of courses'!G35,'-R- List of courses'!G68)</f>
+        <v>60</v>
+      </c>
+      <c r="C2" s="180">
+        <f>SUM('-R- List of courses'!H35,'-R- List of courses'!H68)</f>
+        <v>0</v>
+      </c>
+      <c r="D2" s="180">
+        <f>SUM('-R- List of courses'!I35,'-R- List of courses'!I68)</f>
+        <v>84</v>
+      </c>
+      <c r="E2" s="180">
+        <f>SUM('-R- List of courses'!J35,'-R- List of courses'!J68)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="181" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" s="180">
+        <f>SUM('-R- List of courses'!G36,'-R- List of courses'!G37,'-R- List of courses'!G38,'-R- List of courses'!G69)</f>
+        <v>84</v>
+      </c>
+      <c r="C3" s="180">
+        <f>SUM('-R- List of courses'!H36,'-R- List of courses'!H37,'-R- List of courses'!H38,'-R- List of courses'!H69)</f>
+        <v>0</v>
+      </c>
+      <c r="D3" s="180">
+        <f>SUM('-R- List of courses'!I36,'-R- List of courses'!I37,'-R- List of courses'!I38,'-R- List of courses'!I69)</f>
+        <v>84</v>
+      </c>
+      <c r="E3" s="180">
+        <f>SUM('-R- List of courses'!J36,'-R- List of courses'!J37,'-R- List of courses'!J38,'-R- List of courses'!J69)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="181" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4" s="180">
+        <f>SUM('-R- List of courses'!G39,'-R- List of courses'!G70)</f>
+        <v>24</v>
+      </c>
+      <c r="C4" s="180">
+        <f>SUM('-R- List of courses'!H39,'-R- List of courses'!H70)</f>
+        <v>0</v>
+      </c>
+      <c r="D4" s="180">
+        <f>SUM('-R- List of courses'!I39,'-R- List of courses'!I70)</f>
+        <v>24</v>
+      </c>
+      <c r="E4" s="180">
+        <f>SUM('-R- List of courses'!J39,'-R- List of courses'!J70)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="181" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" s="182">
+        <f>SUM('-R- List of courses'!G40,'-R- List of courses'!G71)</f>
+        <v>0</v>
+      </c>
+      <c r="C5" s="182">
+        <f>SUM('-R- List of courses'!H40,'-R- List of courses'!H71)</f>
+        <v>72</v>
+      </c>
+      <c r="D5" s="182">
+        <f>SUM('-R- List of courses'!I40,'-R- List of courses'!I71)</f>
+        <v>0</v>
+      </c>
+      <c r="E5" s="182">
+        <f>SUM('-R- List of courses'!J40,'-R- List of courses'!J71)</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="181" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" s="182">
+        <f>SUM('-R- List of courses'!G41,'-R- List of courses'!G72)</f>
+        <v>0</v>
+      </c>
+      <c r="C6" s="182">
+        <f>SUM('-R- List of courses'!H41,'-R- List of courses'!H72)</f>
+        <v>72</v>
+      </c>
+      <c r="D6" s="182">
+        <f>SUM('-R- List of courses'!I41,'-R- List of courses'!I72)</f>
+        <v>0</v>
+      </c>
+      <c r="E6" s="182">
+        <f>SUM('-R- List of courses'!J41,'-R- List of courses'!J72)</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="181" t="s">
+        <v>99</v>
+      </c>
+      <c r="B7" s="182">
+        <f>SUM('-R- List of courses'!G80,'-R- List of courses'!G79,'-R- List of courses'!G48,'-R- List of courses'!G47)</f>
+        <v>90</v>
+      </c>
+      <c r="C7" s="182">
+        <f>SUM('-R- List of courses'!H80,'-R- List of courses'!H79,'-R- List of courses'!H48,'-R- List of courses'!H47)</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="182">
+        <f>SUM('-R- List of courses'!I80,'-R- List of courses'!I79,'-R- List of courses'!I48,'-R- List of courses'!I47)</f>
+        <v>81</v>
+      </c>
+      <c r="E7" s="182">
+        <f>SUM('-R- List of courses'!J80,'-R- List of courses'!J79,'-R- List of courses'!J48,'-R- List of courses'!J47)</f>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="181" t="s">
+        <v>98</v>
+      </c>
+      <c r="B8" s="180">
+        <f>SUM('-R- List of courses'!G73)</f>
+        <v>6</v>
+      </c>
+      <c r="C8" s="180">
+        <f>SUM('-R- List of courses'!H73)</f>
+        <v>6</v>
+      </c>
+      <c r="D8" s="180">
+        <f>SUM('-R- List of courses'!I73)</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="180">
+        <f>SUM('-R- List of courses'!J73)</f>
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E29076A-97D4-462D-973F-00B42C393D58}">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="182" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" s="182" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="182" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="182" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="182" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="181" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="180">
+        <f>SUM('-R- List of courses'!G35,'-R- List of courses'!G68)</f>
+        <v>60</v>
+      </c>
+      <c r="C2" s="180">
+        <f>SUM('-R- List of courses'!H35,'-R- List of courses'!H68)</f>
+        <v>0</v>
+      </c>
+      <c r="D2" s="180">
+        <f>SUM('-R- List of courses'!I35,'-R- List of courses'!I68)</f>
+        <v>84</v>
+      </c>
+      <c r="E2" s="180">
+        <f>SUM('-R- List of courses'!J35,'-R- List of courses'!J68)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="181" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" s="180">
+        <f>SUM('-R- List of courses'!G36,'-R- List of courses'!G37,'-R- List of courses'!G38,'-R- List of courses'!G69)</f>
+        <v>84</v>
+      </c>
+      <c r="C3" s="180">
+        <f>SUM('-R- List of courses'!H36,'-R- List of courses'!H37,'-R- List of courses'!H38,'-R- List of courses'!H69)</f>
+        <v>0</v>
+      </c>
+      <c r="D3" s="180">
+        <f>SUM('-R- List of courses'!I36,'-R- List of courses'!I37,'-R- List of courses'!I38,'-R- List of courses'!I69)</f>
+        <v>84</v>
+      </c>
+      <c r="E3" s="180">
+        <f>SUM('-R- List of courses'!J36,'-R- List of courses'!J37,'-R- List of courses'!J38,'-R- List of courses'!J69)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="181" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4" s="180">
+        <f>SUM('-R- List of courses'!G39,'-R- List of courses'!G51,'-R- List of courses'!G52,'-R- List of courses'!G70,'-R- List of courses'!G83,'-R- List of courses'!G84)</f>
+        <v>99</v>
+      </c>
+      <c r="C4" s="180">
+        <f>SUM('-R- List of courses'!H39,'-R- List of courses'!H51,'-R- List of courses'!H52,'-R- List of courses'!H70,'-R- List of courses'!H83,'-R- List of courses'!H84)</f>
+        <v>0</v>
+      </c>
+      <c r="D4" s="180">
+        <f>SUM('-R- List of courses'!I39,'-R- List of courses'!I51,'-R- List of courses'!I52,'-R- List of courses'!I70,'-R- List of courses'!I83,'-R- List of courses'!I84)</f>
+        <v>84</v>
+      </c>
+      <c r="E4" s="180">
+        <f>SUM('-R- List of courses'!J39,'-R- List of courses'!J51,'-R- List of courses'!J52,'-R- List of courses'!J70,'-R- List of courses'!J83,'-R- List of courses'!J84)</f>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="181" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" s="182">
+        <f>SUM('-R- List of courses'!G40,'-R- List of courses'!G71)</f>
+        <v>0</v>
+      </c>
+      <c r="C5" s="182">
+        <f>SUM('-R- List of courses'!H40,'-R- List of courses'!H71)</f>
+        <v>72</v>
+      </c>
+      <c r="D5" s="182">
+        <f>SUM('-R- List of courses'!I40,'-R- List of courses'!I71)</f>
+        <v>0</v>
+      </c>
+      <c r="E5" s="182">
+        <f>SUM('-R- List of courses'!J40,'-R- List of courses'!J71)</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="181" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" s="182">
+        <f>SUM('-R- List of courses'!G41,'-R- List of courses'!G72)</f>
+        <v>0</v>
+      </c>
+      <c r="C6" s="182">
+        <f>SUM('-R- List of courses'!H41,'-R- List of courses'!H72)</f>
+        <v>72</v>
+      </c>
+      <c r="D6" s="182">
+        <f>SUM('-R- List of courses'!I41,'-R- List of courses'!I72)</f>
+        <v>0</v>
+      </c>
+      <c r="E6" s="182">
+        <f>SUM('-R- List of courses'!J41,'-R- List of courses'!J72)</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="181" t="s">
+        <v>99</v>
+      </c>
+      <c r="B7" s="182">
+        <v>0</v>
+      </c>
+      <c r="C7" s="182">
+        <v>0</v>
+      </c>
+      <c r="D7" s="182">
+        <v>0</v>
+      </c>
+      <c r="E7" s="182">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="181" t="s">
+        <v>98</v>
+      </c>
+      <c r="B8" s="180">
+        <f>SUM('-R- List of courses'!G73)</f>
+        <v>6</v>
+      </c>
+      <c r="C8" s="180">
+        <f>SUM('-R- List of courses'!H73)</f>
+        <v>6</v>
+      </c>
+      <c r="D8" s="180">
+        <f>SUM('-R- List of courses'!I73)</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="180">
+        <f>SUM('-R- List of courses'!J73)</f>
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C7547F6-997D-476A-8B57-E60F7008608E}">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="182" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="182" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="182" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="182" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="182" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="181" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="180">
+        <f>SUM('-R- List of courses'!G35,'-R- List of courses'!G68)</f>
+        <v>60</v>
+      </c>
+      <c r="C2" s="180">
+        <f>SUM('-R- List of courses'!H35,'-R- List of courses'!H68)</f>
+        <v>0</v>
+      </c>
+      <c r="D2" s="180">
+        <f>SUM('-R- List of courses'!I35,'-R- List of courses'!I68)</f>
+        <v>84</v>
+      </c>
+      <c r="E2" s="180">
+        <f>SUM('-R- List of courses'!J35,'-R- List of courses'!J68)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="181" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" s="180">
+        <f>SUM('-R- List of courses'!G36,'-R- List of courses'!G37,'-R- List of courses'!G38,'-R- List of courses'!G56,'-R- List of courses'!G69,'-R- List of courses'!G88)</f>
+        <v>84</v>
+      </c>
+      <c r="C3" s="180">
+        <f>SUM('-R- List of courses'!H36,'-R- List of courses'!H37,'-R- List of courses'!H38,'-R- List of courses'!H56,'-R- List of courses'!H69,'-R- List of courses'!H88)</f>
+        <v>60</v>
+      </c>
+      <c r="D3" s="180">
+        <f>SUM('-R- List of courses'!I36,'-R- List of courses'!I37,'-R- List of courses'!I38,'-R- List of courses'!I56,'-R- List of courses'!I69,'-R- List of courses'!I88)</f>
+        <v>84</v>
+      </c>
+      <c r="E3" s="180">
+        <f>SUM('-R- List of courses'!J36,'-R- List of courses'!J37,'-R- List of courses'!J38,'-R- List of courses'!J56,'-R- List of courses'!J69,'-R- List of courses'!J88)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="181" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4" s="180">
+        <f>SUM('-R- List of courses'!G39,'-R- List of courses'!G70)</f>
+        <v>24</v>
+      </c>
+      <c r="C4" s="180">
+        <f>SUM('-R- List of courses'!H39,'-R- List of courses'!H70)</f>
+        <v>0</v>
+      </c>
+      <c r="D4" s="180">
+        <f>SUM('-R- List of courses'!I39,'-R- List of courses'!I70)</f>
+        <v>24</v>
+      </c>
+      <c r="E4" s="180">
+        <f>SUM('-R- List of courses'!J39,'-R- List of courses'!J70)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="181" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" s="182">
+        <f>SUM('-R- List of courses'!G40,'-R- List of courses'!G71)</f>
+        <v>0</v>
+      </c>
+      <c r="C5" s="182">
+        <f>SUM('-R- List of courses'!H40,'-R- List of courses'!H71)</f>
+        <v>72</v>
+      </c>
+      <c r="D5" s="182">
+        <f>SUM('-R- List of courses'!I40,'-R- List of courses'!I71)</f>
+        <v>0</v>
+      </c>
+      <c r="E5" s="182">
+        <f>SUM('-R- List of courses'!J40,'-R- List of courses'!J71)</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="181" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" s="182">
+        <f>SUM('-R- List of courses'!G41,'-R- List of courses'!G72)</f>
+        <v>0</v>
+      </c>
+      <c r="C6" s="182">
+        <f>SUM('-R- List of courses'!H41,'-R- List of courses'!H72)</f>
+        <v>72</v>
+      </c>
+      <c r="D6" s="182">
+        <f>SUM('-R- List of courses'!I41,'-R- List of courses'!I72)</f>
+        <v>0</v>
+      </c>
+      <c r="E6" s="182">
+        <f>SUM('-R- List of courses'!J41,'-R- List of courses'!J72)</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="181" t="s">
+        <v>99</v>
+      </c>
+      <c r="B7" s="182">
+        <f>SUM('-R- List of courses'!G55,'-R- List of courses'!G87)</f>
+        <v>60</v>
+      </c>
+      <c r="C7" s="182">
+        <f>SUM('-R- List of courses'!H55,'-R- List of courses'!H87)</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="182">
+        <f>SUM('-R- List of courses'!I55,'-R- List of courses'!I87)</f>
+        <v>51</v>
+      </c>
+      <c r="E7" s="182">
+        <f>SUM('-R- List of courses'!J55,'-R- List of courses'!J87)</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="181" t="s">
+        <v>98</v>
+      </c>
+      <c r="B8" s="180">
+        <f>SUM('-R- List of courses'!G73)</f>
+        <v>6</v>
+      </c>
+      <c r="C8" s="180">
+        <f>SUM('-R- List of courses'!H73)</f>
+        <v>6</v>
+      </c>
+      <c r="D8" s="180">
+        <f>SUM('-R- List of courses'!I73)</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="180">
+        <f>SUM('-R- List of courses'!J73)</f>
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{472082C4-0291-4619-997B-D46CC335CDAC}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="182" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" s="182" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="182" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="182" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="182" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="181" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="180">
+        <f>SUM('-R- List of courses'!G35,'-R- List of courses'!G68,'-R- List of courses'!G92)</f>
+        <v>75</v>
+      </c>
+      <c r="C2" s="180">
+        <f>SUM('-R- List of courses'!H35,'-R- List of courses'!H68,'-R- List of courses'!H92)</f>
+        <v>0</v>
+      </c>
+      <c r="D2" s="180">
+        <f>SUM('-R- List of courses'!I35,'-R- List of courses'!I68,'-R- List of courses'!I92)</f>
+        <v>90</v>
+      </c>
+      <c r="E2" s="180">
+        <f>SUM('-R- List of courses'!J35,'-R- List of courses'!J68,'-R- List of courses'!J92)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="181" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" s="180">
+        <f>SUM('-R- List of courses'!G36,'-R- List of courses'!G37,'-R- List of courses'!G38,'-R- List of courses'!G60,'-R- List of courses'!G69)</f>
+        <v>99</v>
+      </c>
+      <c r="C3" s="180">
+        <f>SUM('-R- List of courses'!H36,'-R- List of courses'!H37,'-R- List of courses'!H38,'-R- List of courses'!H60,'-R- List of courses'!H69)</f>
+        <v>0</v>
+      </c>
+      <c r="D3" s="180">
+        <f>SUM('-R- List of courses'!I36,'-R- List of courses'!I37,'-R- List of courses'!I38,'-R- List of courses'!I60,'-R- List of courses'!I69)</f>
+        <v>93</v>
+      </c>
+      <c r="E3" s="180">
+        <f>SUM('-R- List of courses'!J36,'-R- List of courses'!J37,'-R- List of courses'!J38,'-R- List of courses'!J60,'-R- List of courses'!J69)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="181" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4" s="180">
+        <f>SUM('-R- List of courses'!G39,'-R- List of courses'!G70)</f>
+        <v>24</v>
+      </c>
+      <c r="C4" s="180">
+        <f>SUM('-R- List of courses'!H39,'-R- List of courses'!H70)</f>
+        <v>0</v>
+      </c>
+      <c r="D4" s="180">
+        <f>SUM('-R- List of courses'!I39,'-R- List of courses'!I70)</f>
+        <v>24</v>
+      </c>
+      <c r="E4" s="180">
+        <f>SUM('-R- List of courses'!J39,'-R- List of courses'!J70)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="181" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" s="182">
+        <f>SUM('-R- List of courses'!G40,'-R- List of courses'!G71)</f>
+        <v>0</v>
+      </c>
+      <c r="C5" s="182">
+        <f>SUM('-R- List of courses'!H40,'-R- List of courses'!H71)</f>
+        <v>72</v>
+      </c>
+      <c r="D5" s="182">
+        <f>SUM('-R- List of courses'!I40,'-R- List of courses'!I71)</f>
+        <v>0</v>
+      </c>
+      <c r="E5" s="182">
+        <f>SUM('-R- List of courses'!J40,'-R- List of courses'!J71)</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="181" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" s="182">
+        <f>SUM('-R- List of courses'!G41,'-R- List of courses'!G72)</f>
+        <v>0</v>
+      </c>
+      <c r="C6" s="182">
+        <f>SUM('-R- List of courses'!H41,'-R- List of courses'!H72)</f>
+        <v>72</v>
+      </c>
+      <c r="D6" s="182">
+        <f>SUM('-R- List of courses'!I41,'-R- List of courses'!I72)</f>
+        <v>0</v>
+      </c>
+      <c r="E6" s="182">
+        <f>SUM('-R- List of courses'!J41,'-R- List of courses'!J72)</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="181" t="s">
+        <v>99</v>
+      </c>
+      <c r="B7" s="182">
+        <f>SUM('-R- List of courses'!G59,'-R- List of courses'!G91)</f>
+        <v>60</v>
+      </c>
+      <c r="C7" s="182">
+        <f>SUM('-R- List of courses'!H59,'-R- List of courses'!H91)</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="182">
+        <f>SUM('-R- List of courses'!I59,'-R- List of courses'!I91)</f>
+        <v>51</v>
+      </c>
+      <c r="E7" s="182">
+        <f>SUM('-R- List of courses'!J59,'-R- List of courses'!J91)</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="181" t="s">
+        <v>98</v>
+      </c>
+      <c r="B8" s="180">
+        <f>SUM('-R- List of courses'!G73)</f>
+        <v>6</v>
+      </c>
+      <c r="C8" s="180">
+        <f>SUM('-R- List of courses'!H73)</f>
+        <v>6</v>
+      </c>
+      <c r="D8" s="180">
+        <f>SUM('-R- List of courses'!I73)</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="180">
+        <f>SUM('-R- List of courses'!J73)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="181"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A483C64F-7CB5-4EC6-9394-026A62F84C7A}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="27.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="181" t="s">
         <v>105</v>
       </c>
-      <c r="B11">
+      <c r="B1" s="182">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="181" t="s">
+    <row r="2" spans="1:2">
+      <c r="A2" s="181" t="s">
         <v>106</v>
       </c>
-      <c r="B12">
+      <c r="B2" s="182">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="181" t="s">
+    <row r="3" spans="1:2">
+      <c r="A3" s="182" t="s">
+        <v>116</v>
+      </c>
+      <c r="B3" s="182">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="181" t="s">
         <v>107</v>
       </c>
-      <c r="B14">
-        <f>B11*SUM('-R- List of courses'!G13:J13,'-R- List of courses'!G27:J27)</f>
+      <c r="B4" s="182">
+        <f>B1*SUM(L0!B2:E8)</f>
         <v>6280</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="181" t="s">
+    <row r="5" spans="1:2">
+      <c r="A5" s="181" t="s">
         <v>108</v>
       </c>
-      <c r="B15">
-        <f>B12 * SUM('-R- List of courses'!G42:J42,'-R- List of courses'!G74:J74)</f>
-        <v>4944</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="181" t="s">
+      <c r="B5" s="182">
+        <f>B3*SUM(L1CE!B2:E8)</f>
+        <v>1722</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="181" t="s">
         <v>109</v>
       </c>
-      <c r="B16">
-        <f>2*SUM('-R- List of courses'!G47:J48,'-R- List of courses'!G79:J80)</f>
-        <v>486</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="181" t="s">
+      <c r="B6" s="182">
+        <f>B3*SUM(L1CS!B2:E8)</f>
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="181" t="s">
         <v>110</v>
       </c>
-      <c r="B17">
-        <f>2*SUM('-R- List of courses'!G83:J84,'-R- List of courses'!G51:J52)</f>
-        <v>384</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="181" t="s">
+      <c r="B7" s="182">
+        <f>B3*SUM(L1GE!B2:E8)</f>
+        <v>1662</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="181" t="s">
         <v>111</v>
       </c>
-      <c r="B18">
-        <f>2*SUM('-R- List of courses'!G55:J56,'-R- List of courses'!G87:J88)</f>
-        <v>426</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="181" t="s">
-        <v>112</v>
-      </c>
-      <c r="B19">
-        <f>2*SUM('-R- List of courses'!G91:J92,'-R- List of courses'!G59:J60)</f>
-        <v>426</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="181" t="s">
+      <c r="B8" s="182">
+        <f>B3*SUM(L1OG!B2:E8)</f>
+        <v>1662</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="181" t="s">
         <v>96</v>
       </c>
-      <c r="B20">
-        <f>SUM(B14:B19)</f>
+      <c r="B9" s="182">
+        <f>SUM(B4:B8)</f>
         <v>12946</v>
       </c>
     </row>

</xml_diff>